<commit_message>
Phase 2b - task 4, 5
</commit_message>
<xml_diff>
--- a/dbt_run_logs/dbt_run_logs_results.xlsx
+++ b/dbt_run_logs/dbt_run_logs_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nauka\studia\sem 10\TBD\projekt\tbd-workshop-1\dbt_run_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AF04CE-0BBB-41FC-A49A-12A82BC32BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894B54AA-01E6-47C6-A422-FF30CC716E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,10 +173,10 @@
     <t>Czas przetwarzania całkowity</t>
   </si>
   <si>
-    <t>Nazwa przetwarzanego modelu tabeli</t>
-  </si>
-  <si>
-    <t>Czas przetwarzania modelu tabeli dla "x" instancji egzekutora [s]</t>
+    <t>Nazwa przetwarzanego modelu</t>
+  </si>
+  <si>
+    <t>Czas przetwarzania modelu dla "x" instancji egzekutora [s]</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL" sz="1800" b="1"/>
-              <a:t>Całkowity czas przetwarzania [s]</a:t>
+              <a:t>Całkowity czas przetwarzania modeli [s]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -940,7 +940,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pl-PL" sz="2000" b="1" baseline="0"/>
-              <a:t> modelu tabeli</a:t>
+              <a:t> modelu</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pl-PL" sz="2000" b="1"/>
@@ -1949,7 +1949,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="pl-PL" sz="2000" b="1" baseline="0"/>
-                  <a:t> modelu tabeli</a:t>
+                  <a:t> modelu</a:t>
                 </a:r>
                 <a:endParaRPr lang="pl-PL" sz="2000" b="1"/>
               </a:p>
@@ -3683,7 +3683,7 @@
   <dimension ref="B4:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="E4" sqref="E4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>